<commit_message>
add weight for category and only matched maximum weight
</commit_message>
<xml_diff>
--- a/classification_matching_2.0/GOOGLE API BUSSINESS TYPE NAMES.xlsx
+++ b/classification_matching_2.0/GOOGLE API BUSSINESS TYPE NAMES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weihongtan/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{28FE2AB5-63CC-4A56-A2AD-715D66A8A5D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5AD483-4AC0-E04F-AA4C-61D8D37CA712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4100" yWindow="500" windowWidth="28800" windowHeight="16240" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="193">
   <si>
     <t>GOOGLE API ALL BUSINESS TYPE</t>
   </si>
@@ -637,6 +637,9 @@
   </si>
   <si>
     <t>Food Production and Preparation</t>
+  </si>
+  <si>
+    <t>Weight</t>
   </si>
 </sst>
 </file>
@@ -1008,19 +1011,19 @@
       <selection activeCell="A69" sqref="A69:XFD69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="52.140625" customWidth="1"/>
+    <col min="1" max="1" width="52.1640625" customWidth="1"/>
     <col min="2" max="2" width="60" customWidth="1"/>
-    <col min="3" max="3" width="45.42578125" customWidth="1"/>
-    <col min="5" max="5" width="42.85546875" customWidth="1"/>
-    <col min="6" max="6" width="28.5703125" customWidth="1"/>
-    <col min="7" max="7" width="124.5703125" customWidth="1"/>
-    <col min="10" max="10" width="31.28515625" customWidth="1"/>
-    <col min="13" max="13" width="61.85546875" customWidth="1"/>
+    <col min="3" max="3" width="45.5" customWidth="1"/>
+    <col min="5" max="5" width="42.83203125" customWidth="1"/>
+    <col min="6" max="6" width="28.5" customWidth="1"/>
+    <col min="7" max="7" width="124.5" customWidth="1"/>
+    <col min="10" max="10" width="31.33203125" customWidth="1"/>
+    <col min="13" max="13" width="61.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15">
+    <row r="1" spans="1:13" ht="16">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1049,7 +1052,7 @@
         <v>1</v>
       </c>
       <c r="M1" t="str">
-        <f>VLOOKUP(J1,A:E,2,TRUE)</f>
+        <f t="shared" ref="M1:M43" si="0">VLOOKUP(J1,A:E,2,TRUE)</f>
         <v>INSTITUTIONAL FOOD</v>
       </c>
     </row>
@@ -1069,11 +1072,11 @@
         <v>1</v>
       </c>
       <c r="M2" t="str">
-        <f>VLOOKUP(J2,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>INSTITUTIONAL FOOD</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15">
+    <row r="3" spans="1:13" ht="16">
       <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
@@ -1102,11 +1105,11 @@
         <v>10</v>
       </c>
       <c r="M3">
-        <f>VLOOKUP(J3,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="45.75">
+    <row r="4" spans="1:13" ht="48">
       <c r="A4" s="6" t="s">
         <v>18</v>
       </c>
@@ -1131,11 +1134,11 @@
         <v>1</v>
       </c>
       <c r="M4" t="str">
-        <f>VLOOKUP(J4,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>FOOD RETAIL</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="36">
+    <row r="5" spans="1:13" ht="42">
       <c r="A5" s="6" t="s">
         <v>24</v>
       </c>
@@ -1160,11 +1163,11 @@
         <v>1</v>
       </c>
       <c r="M5" t="str">
-        <f>VLOOKUP(J5,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>INSTITUTIONAL FOOD</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="36">
+    <row r="6" spans="1:13" ht="42">
       <c r="A6" s="6" t="s">
         <v>26</v>
       </c>
@@ -1189,7 +1192,7 @@
         <v>2</v>
       </c>
       <c r="M6" t="str">
-        <f>VLOOKUP(J6,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>INSTITUTIONAL FOOD</v>
       </c>
     </row>
@@ -1209,7 +1212,7 @@
         <v>1</v>
       </c>
       <c r="M7" t="str">
-        <f>VLOOKUP(J7,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>FOOD SERVICE</v>
       </c>
     </row>
@@ -1238,7 +1241,7 @@
         <v>2</v>
       </c>
       <c r="M8" t="str">
-        <f>VLOOKUP(J8,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>FOOD RETAIL</v>
       </c>
     </row>
@@ -1258,11 +1261,11 @@
         <v>23</v>
       </c>
       <c r="M9" t="str">
-        <f>VLOOKUP(J9,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>FOOD RETAIL</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="24">
+    <row r="10" spans="1:13" ht="28">
       <c r="A10" s="6" t="s">
         <v>37</v>
       </c>
@@ -1291,11 +1294,11 @@
         <v>1</v>
       </c>
       <c r="M10" t="str">
-        <f>VLOOKUP(J10,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>ACCOMMODATION/ RECREATION SERVICES</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="24">
+    <row r="11" spans="1:13" ht="28">
       <c r="A11" s="6" t="s">
         <v>45</v>
       </c>
@@ -1324,11 +1327,11 @@
         <v>1</v>
       </c>
       <c r="M11" t="str">
-        <f>VLOOKUP(J11,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>INSTITUTIONAL FOOD</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="36">
+    <row r="12" spans="1:13" ht="42">
       <c r="A12" s="6" t="s">
         <v>52</v>
       </c>
@@ -1353,11 +1356,11 @@
         <v>1</v>
       </c>
       <c r="M12" t="str">
-        <f>VLOOKUP(J12,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>ACCOMMODATION/ RECREATION SERVICES</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="36">
+    <row r="13" spans="1:13" ht="42">
       <c r="A13" s="6" t="s">
         <v>57</v>
       </c>
@@ -1382,7 +1385,7 @@
         <v>4</v>
       </c>
       <c r="M13" t="str">
-        <f>VLOOKUP(J13,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>FOOD RETAIL</v>
       </c>
     </row>
@@ -1415,11 +1418,11 @@
         <v>1</v>
       </c>
       <c r="M14" t="str">
-        <f>VLOOKUP(J14,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>FOOD SERVICE</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15.75">
+    <row r="15" spans="1:13" ht="16">
       <c r="A15" s="6" t="s">
         <v>63</v>
       </c>
@@ -1448,11 +1451,11 @@
         <v>1</v>
       </c>
       <c r="M15" t="str">
-        <f>VLOOKUP(J15,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>FOOD RETAIL</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="36">
+    <row r="16" spans="1:13" ht="42">
       <c r="A16" s="6" t="s">
         <v>64</v>
       </c>
@@ -1477,7 +1480,7 @@
         <v>5</v>
       </c>
       <c r="M16" t="str">
-        <f>VLOOKUP(J16,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>FOOD RETAIL</v>
       </c>
     </row>
@@ -1503,7 +1506,7 @@
         <v>1</v>
       </c>
       <c r="M17" t="str">
-        <f>VLOOKUP(J17,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>INSTITUTIONAL FOOD</v>
       </c>
     </row>
@@ -1523,7 +1526,7 @@
         <v>2</v>
       </c>
       <c r="M18">
-        <f>VLOOKUP(J18,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1543,7 +1546,7 @@
         <v>1</v>
       </c>
       <c r="M19">
-        <f>VLOOKUP(J19,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1563,7 +1566,7 @@
         <v>1</v>
       </c>
       <c r="M20" t="str">
-        <f>VLOOKUP(J20,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>ACCOMMODATION/ RECREATION SERVICES</v>
       </c>
     </row>
@@ -1583,7 +1586,7 @@
         <v>1</v>
       </c>
       <c r="M21" t="str">
-        <f>VLOOKUP(J21,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>INSTITUTIONAL FOOD</v>
       </c>
     </row>
@@ -1607,7 +1610,7 @@
         <v>4</v>
       </c>
       <c r="M22" t="str">
-        <f>VLOOKUP(J22,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>ACCOMMODATION/ RECREATION SERVICES</v>
       </c>
     </row>
@@ -1627,7 +1630,7 @@
         <v>1</v>
       </c>
       <c r="M23" t="str">
-        <f>VLOOKUP(J23,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>FOOD SERVICE</v>
       </c>
     </row>
@@ -1656,11 +1659,11 @@
         <v>1</v>
       </c>
       <c r="M24">
-        <f>VLOOKUP(J24,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="15.75">
+    <row r="25" spans="1:13" ht="16">
       <c r="A25" s="6" t="s">
         <v>87</v>
       </c>
@@ -1689,7 +1692,7 @@
         <v>3</v>
       </c>
       <c r="M25" t="str">
-        <f>VLOOKUP(J25,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>FOOD SERVICE</v>
       </c>
     </row>
@@ -1715,7 +1718,7 @@
         <v>1</v>
       </c>
       <c r="M26" t="str">
-        <f>VLOOKUP(J26,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>FOOD RETAIL</v>
       </c>
     </row>
@@ -1743,7 +1746,7 @@
         <v>2</v>
       </c>
       <c r="M27" t="str">
-        <f>VLOOKUP(J27,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>FOOD RETAIL</v>
       </c>
     </row>
@@ -1763,7 +1766,7 @@
         <v>1</v>
       </c>
       <c r="M28" t="str">
-        <f>VLOOKUP(J28,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>FOOD RETAIL</v>
       </c>
     </row>
@@ -1783,11 +1786,11 @@
         <v>1</v>
       </c>
       <c r="M29" t="str">
-        <f>VLOOKUP(J29,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>FOOD RETAIL</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="36">
+    <row r="30" spans="1:13" ht="42">
       <c r="A30" s="6" t="s">
         <v>96</v>
       </c>
@@ -1812,11 +1815,11 @@
         <v>1</v>
       </c>
       <c r="M30" t="str">
-        <f>VLOOKUP(J30,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>FOOD PRODUCTION AND PREPARATION</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="24">
+    <row r="31" spans="1:13" ht="28">
       <c r="A31" s="6" t="s">
         <v>78</v>
       </c>
@@ -1841,11 +1844,11 @@
         <v>1</v>
       </c>
       <c r="M31" t="str">
-        <f>VLOOKUP(J31,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>FOOD RETAIL</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="36">
+    <row r="32" spans="1:13" ht="42">
       <c r="A32" s="6" t="s">
         <v>102</v>
       </c>
@@ -1870,7 +1873,7 @@
         <v>4</v>
       </c>
       <c r="M32" t="str">
-        <f>VLOOKUP(J32,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>FOOD RETAIL</v>
       </c>
     </row>
@@ -1890,11 +1893,11 @@
         <v>1</v>
       </c>
       <c r="M33" t="str">
-        <f>VLOOKUP(J33,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>FOOD RETAIL</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="36">
+    <row r="34" spans="1:13" ht="42">
       <c r="A34" s="6" t="s">
         <v>101</v>
       </c>
@@ -1919,11 +1922,11 @@
         <v>1</v>
       </c>
       <c r="M34" t="str">
-        <f>VLOOKUP(J34,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>INSTITUTIONAL FOOD</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="15.75">
+    <row r="35" spans="1:13" ht="16">
       <c r="A35" s="6" t="s">
         <v>106</v>
       </c>
@@ -1952,11 +1955,11 @@
         <v>1</v>
       </c>
       <c r="M35" t="str">
-        <f>VLOOKUP(J35,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>FOOD RETAIL</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="15.75">
+    <row r="36" spans="1:13" ht="16">
       <c r="A36" s="6" t="s">
         <v>108</v>
       </c>
@@ -1985,11 +1988,11 @@
         <v>2</v>
       </c>
       <c r="M36" t="str">
-        <f>VLOOKUP(J36,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>FOOD RETAIL</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="36">
+    <row r="37" spans="1:13" ht="42">
       <c r="A37" s="6" t="s">
         <v>110</v>
       </c>
@@ -2014,11 +2017,11 @@
         <v>2</v>
       </c>
       <c r="M37" t="str">
-        <f>VLOOKUP(J37,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>FOOD RETAIL</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="36">
+    <row r="38" spans="1:13" ht="42">
       <c r="A38" s="6" t="s">
         <v>112</v>
       </c>
@@ -2043,11 +2046,11 @@
         <v>1</v>
       </c>
       <c r="M38">
-        <f>VLOOKUP(J38,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="36">
+    <row r="39" spans="1:13" ht="42">
       <c r="A39" s="6" t="s">
         <v>109</v>
       </c>
@@ -2072,7 +2075,7 @@
         <v>2</v>
       </c>
       <c r="M39" t="str">
-        <f>VLOOKUP(J39,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>FOOD RETAIL</v>
       </c>
     </row>
@@ -2100,7 +2103,7 @@
         <v>1</v>
       </c>
       <c r="M40" t="str">
-        <f>VLOOKUP(J40,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>ACCOMMODATION/ RECREATION SERVICES</v>
       </c>
     </row>
@@ -2128,11 +2131,11 @@
         <v>2</v>
       </c>
       <c r="M41" t="str">
-        <f>VLOOKUP(J41,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>FOOD RETAIL</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="24">
+    <row r="42" spans="1:13" ht="28">
       <c r="A42" s="6" t="s">
         <v>119</v>
       </c>
@@ -2161,11 +2164,11 @@
         <v>6</v>
       </c>
       <c r="M42">
-        <f>VLOOKUP(J42,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="36">
+    <row r="43" spans="1:13" ht="42">
       <c r="A43" s="6" t="s">
         <v>107</v>
       </c>
@@ -2190,11 +2193,11 @@
         <v>1</v>
       </c>
       <c r="M43" t="str">
-        <f>VLOOKUP(J43,A:E,2,TRUE)</f>
+        <f t="shared" si="0"/>
         <v>FOOD RETAIL</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="15">
+    <row r="44" spans="1:13" ht="16">
       <c r="A44" s="6" t="s">
         <v>51</v>
       </c>
@@ -2207,7 +2210,7 @@
       <c r="F44" s="7"/>
       <c r="G44" s="13"/>
     </row>
-    <row r="45" spans="1:13" ht="30.75">
+    <row r="45" spans="1:13" ht="16">
       <c r="A45" s="6" t="s">
         <v>120</v>
       </c>
@@ -2236,7 +2239,7 @@
         <v>FOOD RETAIL</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="36">
+    <row r="46" spans="1:13" ht="42">
       <c r="A46" s="6" t="s">
         <v>103</v>
       </c>
@@ -2265,7 +2268,7 @@
         <v>FOOD RETAIL</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="24">
+    <row r="47" spans="1:13" ht="28">
       <c r="A47" s="6" t="s">
         <v>124</v>
       </c>
@@ -2350,7 +2353,7 @@
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
     </row>
-    <row r="52" spans="1:7" ht="15.75">
+    <row r="52" spans="1:7" ht="16">
       <c r="A52" s="6" t="s">
         <v>129</v>
       </c>
@@ -2389,7 +2392,7 @@
       <c r="E53" s="11"/>
       <c r="F53" s="7"/>
     </row>
-    <row r="54" spans="1:7" ht="15.75">
+    <row r="54" spans="1:7" ht="16">
       <c r="A54" s="6" t="s">
         <v>132</v>
       </c>
@@ -2438,7 +2441,7 @@
       <c r="E56" s="7"/>
       <c r="F56" s="7"/>
     </row>
-    <row r="57" spans="1:7" ht="48">
+    <row r="57" spans="1:7" ht="56">
       <c r="A57" s="6" t="s">
         <v>97</v>
       </c>
@@ -2489,7 +2492,7 @@
       <c r="E59" s="7"/>
       <c r="F59" s="7"/>
     </row>
-    <row r="60" spans="1:7" ht="36">
+    <row r="60" spans="1:7" ht="42">
       <c r="A60" s="6" t="s">
         <v>142</v>
       </c>
@@ -2550,7 +2553,7 @@
       <c r="E63" s="7"/>
       <c r="F63" s="7"/>
     </row>
-    <row r="64" spans="1:7" ht="24">
+    <row r="64" spans="1:7" ht="28">
       <c r="A64" s="6" t="s">
         <v>145</v>
       </c>
@@ -2606,7 +2609,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="60">
+    <row r="67" spans="1:7" ht="70">
       <c r="A67" s="7" t="s">
         <v>113</v>
       </c>
@@ -2625,7 +2628,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="36">
+    <row r="68" spans="1:7" ht="42">
       <c r="A68" s="6" t="s">
         <v>151</v>
       </c>
@@ -2651,7 +2654,7 @@
       <c r="F69" s="7"/>
       <c r="G69" s="13"/>
     </row>
-    <row r="70" spans="1:7" ht="36">
+    <row r="70" spans="1:7" ht="42">
       <c r="A70" s="6" t="s">
         <v>152</v>
       </c>
@@ -2706,7 +2709,7 @@
       <c r="E73" s="7"/>
       <c r="F73" s="7"/>
     </row>
-    <row r="74" spans="1:7" ht="24">
+    <row r="74" spans="1:7" ht="28">
       <c r="A74" s="6" t="s">
         <v>155</v>
       </c>
@@ -2745,7 +2748,7 @@
       <c r="E75" s="8"/>
       <c r="F75" s="8"/>
     </row>
-    <row r="76" spans="1:7" ht="24">
+    <row r="76" spans="1:7" ht="28">
       <c r="A76" s="6" t="s">
         <v>7</v>
       </c>
@@ -2832,7 +2835,7 @@
       <c r="E81" s="7"/>
       <c r="F81" s="7"/>
     </row>
-    <row r="82" spans="1:7" ht="24">
+    <row r="82" spans="1:7" ht="28">
       <c r="A82" s="6" t="s">
         <v>25</v>
       </c>
@@ -2855,7 +2858,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="36">
+    <row r="83" spans="1:7" ht="42">
       <c r="A83" s="6" t="s">
         <v>169</v>
       </c>
@@ -2884,7 +2887,7 @@
       <c r="E84" s="7"/>
       <c r="F84" s="7"/>
     </row>
-    <row r="85" spans="1:7" ht="24">
+    <row r="85" spans="1:7" ht="28">
       <c r="A85" s="6" t="s">
         <v>76</v>
       </c>
@@ -2951,7 +2954,7 @@
       <c r="E88" s="7"/>
       <c r="F88" s="7"/>
     </row>
-    <row r="89" spans="1:7" ht="24">
+    <row r="89" spans="1:7" ht="28">
       <c r="A89" s="6" t="s">
         <v>174</v>
       </c>
@@ -2974,7 +2977,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="24">
+    <row r="90" spans="1:7" ht="28">
       <c r="A90" s="6" t="s">
         <v>118</v>
       </c>
@@ -3005,7 +3008,7 @@
       <c r="E91" s="7"/>
       <c r="F91" s="7"/>
     </row>
-    <row r="92" spans="1:7" ht="15.75">
+    <row r="92" spans="1:7" ht="16">
       <c r="A92" s="6" t="s">
         <v>180</v>
       </c>
@@ -3044,7 +3047,7 @@
       <c r="E93" s="7"/>
       <c r="F93" s="7"/>
     </row>
-    <row r="94" spans="1:7" ht="15.75">
+    <row r="94" spans="1:7" ht="16">
       <c r="A94" s="6" t="s">
         <v>182</v>
       </c>
@@ -3067,7 +3070,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="15.75">
+    <row r="95" spans="1:7" ht="16">
       <c r="A95" s="6" t="s">
         <v>183</v>
       </c>
@@ -3106,7 +3109,7 @@
       <c r="E96" s="7"/>
       <c r="F96" s="7"/>
     </row>
-    <row r="97" spans="1:7" ht="24">
+    <row r="97" spans="1:7" ht="28">
       <c r="A97" s="6" t="s">
         <v>27</v>
       </c>
@@ -3155,7 +3158,7 @@
       <c r="E99" s="7"/>
       <c r="F99" s="7"/>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:7" ht="14">
       <c r="A100" s="7"/>
       <c r="B100" s="4"/>
       <c r="C100" s="7"/>
@@ -3163,7 +3166,7 @@
       <c r="E100" s="7"/>
       <c r="F100" s="7"/>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:7" ht="14">
       <c r="A101" s="7"/>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
@@ -3171,7 +3174,7 @@
       <c r="E101" s="7"/>
       <c r="F101" s="7"/>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:7" ht="14">
       <c r="A102" s="7"/>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
@@ -3186,1480 +3189,1714 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9EBE679-0237-40D7-B496-4CDAC14B8EDC}">
-  <dimension ref="A1:G78"/>
+  <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A49" sqref="A29:A49"/>
+    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="52.140625" customWidth="1"/>
-    <col min="2" max="2" width="60" customWidth="1"/>
-    <col min="3" max="3" width="45.42578125" customWidth="1"/>
-    <col min="4" max="4" width="35.7109375" customWidth="1"/>
-    <col min="5" max="5" width="42.85546875" customWidth="1"/>
-    <col min="6" max="6" width="28.5703125" customWidth="1"/>
-    <col min="7" max="7" width="124.5703125" customWidth="1"/>
+    <col min="2" max="2" width="52.1640625" customWidth="1"/>
+    <col min="3" max="3" width="60" customWidth="1"/>
+    <col min="4" max="4" width="45.5" customWidth="1"/>
+    <col min="5" max="5" width="35.6640625" customWidth="1"/>
+    <col min="6" max="6" width="42.83203125" customWidth="1"/>
+    <col min="7" max="7" width="28.5" customWidth="1"/>
+    <col min="8" max="8" width="124.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:8" ht="16">
+      <c r="A1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:8" ht="16">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>11</v>
-      </c>
       <c r="C2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="45.75">
-      <c r="A3" s="16" t="s">
+    <row r="3" spans="1:8" ht="48">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="7"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="7"/>
+      <c r="H3" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="36">
-      <c r="A4" s="16" t="s">
+    <row r="4" spans="1:8" ht="42">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="7"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="7"/>
+      <c r="H4" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="36">
-      <c r="A5" s="16" t="s">
+    <row r="5" spans="1:8" ht="42">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="7"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="7"/>
+      <c r="H5" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15">
-      <c r="A6" s="16" t="s">
+    <row r="6" spans="1:8" ht="15">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="C6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="7"/>
       <c r="F6" s="7"/>
-      <c r="G6" t="s">
+      <c r="G6" s="7"/>
+      <c r="H6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="24">
-      <c r="A7" s="16" t="s">
+    <row r="7" spans="1:8" ht="28">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="C7" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="D7" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="E7" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="F7" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="G7" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="H7" s="13" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="24">
-      <c r="A8" s="16" t="s">
+    <row r="8" spans="1:8" ht="28">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="H8" s="13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="36">
-      <c r="A9" s="16" t="s">
+    <row r="9" spans="1:8" ht="42">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>11</v>
-      </c>
       <c r="C9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="E9" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="7"/>
       <c r="F9" s="7"/>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="7"/>
+      <c r="H9" s="13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="36">
-      <c r="A10" s="16" t="s">
+    <row r="10" spans="1:8" ht="42">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>11</v>
-      </c>
       <c r="C10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="E10" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="7"/>
       <c r="F10" s="7"/>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="7"/>
+      <c r="H10" s="13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15">
-      <c r="A11" s="16" t="s">
+    <row r="11" spans="1:8" ht="15">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="C11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="D11" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="F11" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="G11" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75">
-      <c r="A12" s="16" t="s">
+    <row r="12" spans="1:8" ht="16">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>11</v>
-      </c>
       <c r="C12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="E12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="F12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="G12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="H12" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="36">
-      <c r="A13" s="16" t="s">
+    <row r="13" spans="1:8" ht="42">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="D13" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E13" s="7"/>
       <c r="F13" s="7"/>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="7"/>
+      <c r="H13" s="13" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15">
-      <c r="A14" s="16" t="s">
+    <row r="14" spans="1:8" ht="15">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="C14" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="D14" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="E14" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="7"/>
       <c r="F14" s="7"/>
-    </row>
-    <row r="15" spans="1:7" ht="15">
-      <c r="A15" s="16" t="s">
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:8" ht="15">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="D15" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
-    </row>
-    <row r="16" spans="1:7" ht="15">
-      <c r="A16" s="16" t="s">
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:8" ht="15">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="C16" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="D16" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="E16" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="E16" s="7"/>
       <c r="F16" s="7"/>
-      <c r="G16" t="s">
+      <c r="G16" s="7"/>
+      <c r="H16" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75">
-      <c r="A17" s="16" t="s">
+    <row r="17" spans="1:8" ht="16">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>11</v>
-      </c>
       <c r="C17" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="E17" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="F17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="G17" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="12" t="s">
+      <c r="H17" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15">
-      <c r="A18" s="16" t="s">
+    <row r="18" spans="1:8" ht="15">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>11</v>
-      </c>
       <c r="C18" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="E18" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E18" s="7"/>
       <c r="F18" s="7"/>
-    </row>
-    <row r="19" spans="1:7" ht="15">
-      <c r="A19" s="16" t="s">
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:8" ht="15">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="C19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="E19" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="F19" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="F19" s="7"/>
-    </row>
-    <row r="20" spans="1:7" ht="36">
-      <c r="A20" s="16" t="s">
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" ht="42">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="C20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="E20" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E20" s="7"/>
       <c r="F20" s="7"/>
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="7"/>
+      <c r="H20" s="13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="24">
-      <c r="A21" s="16" t="s">
+    <row r="21" spans="1:8" ht="28">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="C21" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="D21" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="E21" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="E21" s="7"/>
       <c r="F21" s="7"/>
-      <c r="G21" s="13" t="s">
+      <c r="G21" s="7"/>
+      <c r="H21" s="13" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="36">
-      <c r="A22" s="16" t="s">
+    <row r="22" spans="1:8" ht="42">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="B22" s="9" t="s">
-        <v>11</v>
-      </c>
       <c r="C22" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="E22" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="7"/>
       <c r="F22" s="7"/>
-      <c r="G22" s="13" t="s">
+      <c r="G22" s="7"/>
+      <c r="H22" s="13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="36">
-      <c r="A23" s="16" t="s">
+    <row r="23" spans="1:8" ht="42">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="B23" s="8" t="s">
-        <v>11</v>
-      </c>
       <c r="C23" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="E23" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E23" s="7"/>
       <c r="F23" s="7"/>
-      <c r="G23" s="13" t="s">
+      <c r="G23" s="7"/>
+      <c r="H23" s="13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75">
-      <c r="A24" s="16" t="s">
+    <row r="24" spans="1:8" ht="16">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="B24" s="8" t="s">
-        <v>11</v>
-      </c>
       <c r="C24" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="E24" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="F24" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F24" s="8" t="s">
+      <c r="G24" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G24" s="12" t="s">
+      <c r="H24" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75">
-      <c r="A25" s="16" t="s">
+    <row r="25" spans="1:8" ht="16">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>11</v>
-      </c>
       <c r="C25" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="E25" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="F25" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="G25" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G25" s="12" t="s">
+      <c r="H25" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="36">
-      <c r="A26" s="16" t="s">
+    <row r="26" spans="1:8" ht="42">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="B26" s="9" t="s">
-        <v>11</v>
-      </c>
       <c r="C26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="E26" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E26" s="7"/>
       <c r="F26" s="7"/>
-      <c r="G26" s="13" t="s">
+      <c r="G26" s="7"/>
+      <c r="H26" s="13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="36">
-      <c r="A27" s="16" t="s">
+    <row r="27" spans="1:8" ht="42">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="B27" s="8" t="s">
-        <v>11</v>
-      </c>
       <c r="C27" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="E27" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E27" s="7"/>
       <c r="F27" s="7"/>
-      <c r="G27" s="13" t="s">
+      <c r="G27" s="7"/>
+      <c r="H27" s="13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="36">
-      <c r="A28" s="16" t="s">
+    <row r="28" spans="1:8" ht="42">
+      <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="B28" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="B28" s="8" t="s">
-        <v>11</v>
-      </c>
       <c r="C28" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="E28" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E28" s="7"/>
       <c r="F28" s="7"/>
-      <c r="G28" s="13" t="s">
+      <c r="G28" s="7"/>
+      <c r="H28" s="13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15">
-      <c r="A29" s="16" t="s">
+    <row r="29" spans="1:8" ht="15">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="C29" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="E29" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="F29" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="F29" s="7"/>
-    </row>
-    <row r="30" spans="1:7" ht="15">
-      <c r="A30" s="16" t="s">
+      <c r="G29" s="7"/>
+    </row>
+    <row r="30" spans="1:8" ht="15">
+      <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="C30" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="D30" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="E30" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="F30" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F30" s="7"/>
-    </row>
-    <row r="31" spans="1:7" ht="24">
-      <c r="A31" s="16" t="s">
+      <c r="G30" s="7"/>
+    </row>
+    <row r="31" spans="1:8" ht="28">
+      <c r="A31">
+        <v>3</v>
+      </c>
+      <c r="B31" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="C31" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="D31" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>47</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="F31" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="G31" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G31" s="13" t="s">
+      <c r="H31" s="13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="36">
-      <c r="A32" s="16" t="s">
+    <row r="32" spans="1:8" ht="42">
+      <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="B32" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="B32" s="9" t="s">
-        <v>11</v>
-      </c>
       <c r="C32" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="E32" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E32" s="7"/>
       <c r="F32" s="7"/>
-      <c r="G32" s="13" t="s">
+      <c r="G32" s="7"/>
+      <c r="H32" s="13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15">
-      <c r="A33" s="16" t="s">
+    <row r="33" spans="1:8" ht="16">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C33" s="9"/>
       <c r="D33" s="9"/>
-      <c r="E33" s="7"/>
+      <c r="E33" s="9"/>
       <c r="F33" s="7"/>
-      <c r="G33" s="13"/>
-    </row>
-    <row r="34" spans="1:7" ht="30.75">
-      <c r="A34" s="16" t="s">
+      <c r="G33" s="7"/>
+      <c r="H33" s="13"/>
+    </row>
+    <row r="34" spans="1:8" ht="16">
+      <c r="A34">
+        <v>5</v>
+      </c>
+      <c r="B34" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="C34" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="D34" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="E34" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="E34" s="7"/>
       <c r="F34" s="7"/>
-      <c r="G34" s="3" t="s">
+      <c r="G34" s="7"/>
+      <c r="H34" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="36">
-      <c r="A35" s="16" t="s">
+    <row r="35" spans="1:8" ht="42">
+      <c r="A35">
+        <v>3</v>
+      </c>
+      <c r="B35" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="B35" s="8" t="s">
-        <v>11</v>
-      </c>
       <c r="C35" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="E35" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E35" s="7"/>
       <c r="F35" s="7"/>
-      <c r="G35" s="13" t="s">
+      <c r="G35" s="7"/>
+      <c r="H35" s="13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="24">
-      <c r="A36" s="16" t="s">
+    <row r="36" spans="1:8" ht="28">
+      <c r="A36">
+        <v>4</v>
+      </c>
+      <c r="B36" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="C36" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="D36" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="E36" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E36" s="7"/>
       <c r="F36" s="7"/>
-      <c r="G36" s="13" t="s">
+      <c r="G36" s="7"/>
+      <c r="H36" s="13" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15">
-      <c r="A37" s="16" t="s">
+    <row r="37" spans="1:8" ht="15">
+      <c r="A37">
+        <v>3</v>
+      </c>
+      <c r="B37" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="C37" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="D37" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="E37" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E37" s="7"/>
       <c r="F37" s="7"/>
-    </row>
-    <row r="38" spans="1:7" ht="15.75">
-      <c r="A38" s="16" t="s">
+      <c r="G37" s="7"/>
+    </row>
+    <row r="38" spans="1:8" ht="16">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="B38" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="B38" s="8" t="s">
-        <v>11</v>
-      </c>
       <c r="C38" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="E38" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="F38" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F38" s="8" t="s">
+      <c r="G38" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G38" s="12" t="s">
+      <c r="H38" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15">
-      <c r="A39" s="16" t="s">
+    <row r="39" spans="1:8" ht="15">
+      <c r="A39">
+        <v>5</v>
+      </c>
+      <c r="B39" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C39" s="10" t="s">
+      <c r="C39" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="E39" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="E39" s="11"/>
-      <c r="F39" s="7"/>
-    </row>
-    <row r="40" spans="1:7" ht="15.75">
-      <c r="A40" s="16" t="s">
+      <c r="F39" s="11"/>
+      <c r="G39" s="7"/>
+    </row>
+    <row r="40" spans="1:8" ht="16">
+      <c r="A40">
+        <v>2</v>
+      </c>
+      <c r="B40" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="B40" s="8" t="s">
-        <v>11</v>
-      </c>
       <c r="C40" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="E40" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E40" s="8" t="s">
+      <c r="F40" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F40" s="8" t="s">
+      <c r="G40" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G40" s="12" t="s">
+      <c r="H40" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15">
-      <c r="A41" s="16" t="s">
+    <row r="41" spans="1:8" ht="15">
+      <c r="A41">
+        <v>2</v>
+      </c>
+      <c r="B41" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="C41" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="D41" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="E41" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="E41" s="7"/>
       <c r="F41" s="7"/>
-    </row>
-    <row r="42" spans="1:7" ht="48">
-      <c r="A42" s="16" t="s">
+      <c r="G41" s="7"/>
+    </row>
+    <row r="42" spans="1:8" ht="56">
+      <c r="A42">
+        <v>3</v>
+      </c>
+      <c r="B42" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="C42" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="D42" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="E42" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="E42" s="7"/>
       <c r="F42" s="7"/>
-      <c r="G42" s="13" t="s">
+      <c r="G42" s="7"/>
+      <c r="H42" s="13" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="15">
-      <c r="A43" s="16" t="s">
+    <row r="43" spans="1:8" ht="15">
+      <c r="A43">
+        <v>3</v>
+      </c>
+      <c r="B43" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="C43" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="D43" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="E43" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="E43" s="7"/>
       <c r="F43" s="7"/>
-    </row>
-    <row r="44" spans="1:7" ht="15">
-      <c r="A44" s="16" t="s">
+      <c r="G43" s="7"/>
+    </row>
+    <row r="44" spans="1:8" ht="15">
+      <c r="A44">
+        <v>5</v>
+      </c>
+      <c r="B44" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="C44" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="D44" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="E44" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="E44" s="7"/>
       <c r="F44" s="7"/>
-    </row>
-    <row r="45" spans="1:7" ht="36">
-      <c r="A45" s="16" t="s">
+      <c r="G44" s="7"/>
+    </row>
+    <row r="45" spans="1:8" ht="42">
+      <c r="A45">
+        <v>3</v>
+      </c>
+      <c r="B45" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="B45" s="8" t="s">
-        <v>11</v>
-      </c>
       <c r="C45" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="E45" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E45" s="7"/>
       <c r="F45" s="7"/>
-      <c r="G45" s="13" t="s">
+      <c r="G45" s="7"/>
+      <c r="H45" s="13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="15">
-      <c r="A46" s="16" t="s">
+    <row r="46" spans="1:8" ht="15">
+      <c r="A46">
+        <v>5</v>
+      </c>
+      <c r="B46" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="C46" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="D46" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="E46" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E46" s="7"/>
       <c r="F46" s="7"/>
-    </row>
-    <row r="47" spans="1:7" ht="15">
-      <c r="A47" s="16" t="s">
+      <c r="G46" s="7"/>
+    </row>
+    <row r="47" spans="1:8" ht="15">
+      <c r="A47">
+        <v>2</v>
+      </c>
+      <c r="B47" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
       <c r="F47" s="7"/>
-    </row>
-    <row r="48" spans="1:7" ht="15">
-      <c r="A48" s="16" t="s">
+      <c r="G47" s="7"/>
+    </row>
+    <row r="48" spans="1:8" ht="15">
+      <c r="A48">
+        <v>4</v>
+      </c>
+      <c r="B48" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="C48" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="D48" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="E48" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E48" s="7"/>
       <c r="F48" s="7"/>
-    </row>
-    <row r="49" spans="1:7" ht="24">
-      <c r="A49" s="16" t="s">
+      <c r="G48" s="7"/>
+    </row>
+    <row r="49" spans="1:8" ht="28">
+      <c r="A49">
+        <v>5</v>
+      </c>
+      <c r="B49" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="C49" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C49" s="8" t="s">
+      <c r="D49" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D49" s="8" t="s">
+      <c r="E49" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E49" s="8" t="s">
+      <c r="F49" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="F49" s="8" t="s">
+      <c r="G49" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="G49" s="13" t="s">
+      <c r="H49" s="13" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="15">
-      <c r="A50" s="6" t="s">
+    <row r="50" spans="1:8" ht="15">
+      <c r="A50">
+        <v>3</v>
+      </c>
+      <c r="B50" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="C50" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="D50" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D50" s="8" t="s">
+      <c r="E50" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E50" s="8" t="s">
+      <c r="F50" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F50" s="8" t="s">
+      <c r="G50" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="G50" t="s">
+      <c r="H50" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="60">
-      <c r="A51" s="7" t="s">
+    <row r="51" spans="1:8" ht="70">
+      <c r="A51">
+        <v>3</v>
+      </c>
+      <c r="B51" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="C51" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="D51" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="D51" s="8" t="s">
+      <c r="E51" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="E51" s="8"/>
       <c r="F51" s="8"/>
-      <c r="G51" s="13" t="s">
+      <c r="G51" s="8"/>
+      <c r="H51" s="13" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="36">
-      <c r="A52" s="6" t="s">
+    <row r="52" spans="1:8" ht="42">
+      <c r="A52">
+        <v>2</v>
+      </c>
+      <c r="B52" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="B52" s="9" t="s">
-        <v>11</v>
-      </c>
       <c r="C52" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D52" s="9" t="s">
+      <c r="E52" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E52" s="7"/>
       <c r="F52" s="7"/>
-      <c r="G52" s="13" t="s">
+      <c r="G52" s="7"/>
+      <c r="H52" s="13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="15">
-      <c r="A53" s="6" t="s">
+    <row r="53" spans="1:8" ht="15">
+      <c r="A53">
+        <v>2</v>
+      </c>
+      <c r="B53" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B53" s="9" t="s">
+      <c r="C53" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C53" s="9"/>
       <c r="D53" s="9"/>
-      <c r="E53" s="7"/>
+      <c r="E53" s="9"/>
       <c r="F53" s="7"/>
-      <c r="G53" s="13"/>
-    </row>
-    <row r="54" spans="1:7" ht="15">
-      <c r="A54" s="6" t="s">
+      <c r="G53" s="7"/>
+      <c r="H53" s="13"/>
+    </row>
+    <row r="54" spans="1:8" ht="15">
+      <c r="A54">
+        <v>2</v>
+      </c>
+      <c r="B54" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B54" s="9" t="s">
-        <v>11</v>
-      </c>
       <c r="C54" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D54" s="9" t="s">
+      <c r="E54" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E54" s="7"/>
       <c r="F54" s="7"/>
-    </row>
-    <row r="55" spans="1:7" ht="24">
-      <c r="A55" s="6" t="s">
+      <c r="G54" s="7"/>
+    </row>
+    <row r="55" spans="1:8" ht="28">
+      <c r="A55">
+        <v>2</v>
+      </c>
+      <c r="B55" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="B55" s="8" t="s">
-        <v>11</v>
-      </c>
       <c r="C55" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D55" s="8" t="s">
+      <c r="E55" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E55" s="8" t="s">
+      <c r="F55" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F55" s="8" t="s">
+      <c r="G55" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G55" s="13" t="s">
+      <c r="H55" s="13" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="15">
-      <c r="A56" s="6" t="s">
+    <row r="56" spans="1:8" ht="15">
+      <c r="A56">
+        <v>2</v>
+      </c>
+      <c r="B56" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="B56" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="C56" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="E56" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E56" s="8"/>
       <c r="F56" s="8"/>
-    </row>
-    <row r="57" spans="1:7" ht="24">
-      <c r="A57" s="6" t="s">
+      <c r="G56" s="8"/>
+    </row>
+    <row r="57" spans="1:8" ht="28">
+      <c r="A57">
+        <v>5</v>
+      </c>
+      <c r="B57" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="C57" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C57" s="10" t="s">
+      <c r="D57" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="D57" s="8" t="s">
+      <c r="E57" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="E57" s="10" t="s">
+      <c r="F57" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="F57" s="10" t="s">
+      <c r="G57" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="G57" s="13" t="s">
+      <c r="H57" s="13" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="15">
-      <c r="A58" s="6" t="s">
+    <row r="58" spans="1:8" ht="15">
+      <c r="A58">
+        <v>3</v>
+      </c>
+      <c r="B58" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="C58" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="D58" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="D58" s="7"/>
       <c r="E58" s="7"/>
       <c r="F58" s="7"/>
-    </row>
-    <row r="59" spans="1:7" ht="15">
-      <c r="A59" s="6" t="s">
+      <c r="G58" s="7"/>
+    </row>
+    <row r="59" spans="1:8" ht="15">
+      <c r="A59">
+        <v>3</v>
+      </c>
+      <c r="B59" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="C59" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C59" s="8" t="s">
+      <c r="D59" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D59" s="8" t="s">
+      <c r="E59" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E59" s="7"/>
       <c r="F59" s="7"/>
-    </row>
-    <row r="60" spans="1:7" ht="15">
-      <c r="A60" s="6" t="s">
+      <c r="G59" s="7"/>
+    </row>
+    <row r="60" spans="1:8" ht="15">
+      <c r="A60">
+        <v>4</v>
+      </c>
+      <c r="B60" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="C60" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C60" s="10" t="s">
+      <c r="D60" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="D60" s="7"/>
       <c r="E60" s="7"/>
       <c r="F60" s="7"/>
-    </row>
-    <row r="61" spans="1:7" ht="24">
-      <c r="A61" s="6" t="s">
+      <c r="G60" s="7"/>
+    </row>
+    <row r="61" spans="1:8" ht="28">
+      <c r="A61">
+        <v>5</v>
+      </c>
+      <c r="B61" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="C61" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C61" s="10" t="s">
+      <c r="D61" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="D61" s="8" t="s">
+      <c r="E61" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="E61" s="10" t="s">
+      <c r="F61" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="F61" s="10" t="s">
+      <c r="G61" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="G61" s="13" t="s">
+      <c r="H61" s="13" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="36">
-      <c r="A62" s="6" t="s">
+    <row r="62" spans="1:8" ht="42">
+      <c r="A62">
+        <v>3</v>
+      </c>
+      <c r="B62" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="B62" s="9" t="s">
-        <v>11</v>
-      </c>
       <c r="C62" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D62" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D62" s="9" t="s">
+      <c r="E62" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E62" s="7"/>
       <c r="F62" s="7"/>
-      <c r="G62" s="13" t="s">
+      <c r="G62" s="7"/>
+      <c r="H62" s="13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="24">
-      <c r="A63" s="6" t="s">
+    <row r="63" spans="1:8" ht="28">
+      <c r="A63">
+        <v>3</v>
+      </c>
+      <c r="B63" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="C63" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C63" s="5" t="s">
+      <c r="D63" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D63" s="8" t="s">
+      <c r="E63" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E63" s="5" t="s">
+      <c r="F63" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F63" s="5" t="s">
+      <c r="G63" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G63" s="13" t="s">
+      <c r="H63" s="13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="15">
-      <c r="A64" s="6" t="s">
+    <row r="64" spans="1:8" ht="15">
+      <c r="A64">
+        <v>3</v>
+      </c>
+      <c r="B64" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="B64" s="8" t="s">
+      <c r="C64" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C64" s="8" t="s">
+      <c r="D64" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D64" s="8" t="s">
+      <c r="E64" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E64" s="7"/>
       <c r="F64" s="7"/>
-    </row>
-    <row r="65" spans="1:7" ht="15">
-      <c r="A65" s="6" t="s">
+      <c r="G64" s="7"/>
+    </row>
+    <row r="65" spans="1:8" ht="15">
+      <c r="A65">
+        <v>5</v>
+      </c>
+      <c r="B65" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="B65" s="8" t="s">
+      <c r="C65" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="C65" s="8" t="s">
+      <c r="D65" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="D65" s="8" t="s">
+      <c r="E65" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="E65" s="8"/>
       <c r="F65" s="8"/>
-    </row>
-    <row r="66" spans="1:7" ht="15">
-      <c r="A66" s="6" t="s">
+      <c r="G65" s="8"/>
+    </row>
+    <row r="66" spans="1:8" ht="15">
+      <c r="A66">
+        <v>4</v>
+      </c>
+      <c r="B66" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B66" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C66" s="7"/>
+      <c r="C66" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="D66" s="7"/>
       <c r="E66" s="7"/>
       <c r="F66" s="7"/>
-    </row>
-    <row r="67" spans="1:7" ht="24">
-      <c r="A67" s="14" t="s">
+      <c r="G66" s="7"/>
+    </row>
+    <row r="67" spans="1:8" ht="28">
+      <c r="A67">
+        <v>3</v>
+      </c>
+      <c r="B67" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="B67" s="8" t="s">
-        <v>11</v>
-      </c>
       <c r="C67" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D67" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D67" s="8" t="s">
+      <c r="E67" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E67" s="8" t="s">
+      <c r="F67" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F67" s="8" t="s">
+      <c r="G67" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G67" s="13" t="s">
+      <c r="H67" s="13" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="24">
-      <c r="A68" s="14" t="s">
+    <row r="68" spans="1:8" ht="28">
+      <c r="A68">
+        <v>5</v>
+      </c>
+      <c r="B68" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="B68" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="C68" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D68" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="D68" s="7"/>
-      <c r="E68" s="5" t="s">
+      <c r="E68" s="7"/>
+      <c r="F68" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="F68" s="5" t="s">
+      <c r="G68" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="G68" s="13" t="s">
+      <c r="H68" s="13" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="15.75">
-      <c r="A69" s="14" t="s">
+    <row r="69" spans="1:8" ht="16">
+      <c r="A69">
+        <v>3</v>
+      </c>
+      <c r="B69" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="B69" s="8" t="s">
-        <v>11</v>
-      </c>
       <c r="C69" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D69" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D69" s="8" t="s">
+      <c r="E69" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E69" s="8" t="s">
+      <c r="F69" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F69" s="8" t="s">
+      <c r="G69" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G69" s="12" t="s">
+      <c r="H69" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="15">
-      <c r="A70" s="14" t="s">
+    <row r="70" spans="1:8" ht="15">
+      <c r="A70">
+        <v>3</v>
+      </c>
+      <c r="B70" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="C70" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C70" s="5" t="s">
+      <c r="D70" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D70" s="5" t="s">
+      <c r="E70" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E70" s="7"/>
       <c r="F70" s="7"/>
-    </row>
-    <row r="71" spans="1:7" ht="15.75">
-      <c r="A71" s="14" t="s">
+      <c r="G70" s="7"/>
+    </row>
+    <row r="71" spans="1:8" ht="16">
+      <c r="A71">
+        <v>3</v>
+      </c>
+      <c r="B71" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="B71" s="8" t="s">
-        <v>11</v>
-      </c>
       <c r="C71" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D71" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D71" s="8" t="s">
+      <c r="E71" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E71" s="8" t="s">
+      <c r="F71" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F71" s="8" t="s">
+      <c r="G71" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G71" s="12" t="s">
+      <c r="H71" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="15.75">
-      <c r="A72" s="14" t="s">
+    <row r="72" spans="1:8" ht="16">
+      <c r="A72">
+        <v>3</v>
+      </c>
+      <c r="B72" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="B72" s="8" t="s">
-        <v>11</v>
-      </c>
       <c r="C72" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D72" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D72" s="8" t="s">
+      <c r="E72" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E72" s="8" t="s">
+      <c r="F72" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F72" s="8" t="s">
+      <c r="G72" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G72" s="12" t="s">
+      <c r="H72" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="15">
-      <c r="A73" s="14" t="s">
+    <row r="73" spans="1:8" ht="15">
+      <c r="A73">
+        <v>3</v>
+      </c>
+      <c r="B73" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="C73" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C73" s="5" t="s">
+      <c r="D73" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D73" s="5" t="s">
+      <c r="E73" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E73" s="7"/>
       <c r="F73" s="7"/>
-    </row>
-    <row r="74" spans="1:7" ht="24">
-      <c r="A74" s="14" t="s">
+      <c r="G73" s="7"/>
+    </row>
+    <row r="74" spans="1:8" ht="28">
+      <c r="A74">
+        <v>5</v>
+      </c>
+      <c r="B74" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="C74" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C74" s="10" t="s">
+      <c r="D74" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="D74" s="8" t="s">
+      <c r="E74" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="E74" s="10" t="s">
+      <c r="F74" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="F74" s="10" t="s">
+      <c r="G74" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="G74" s="13" t="s">
+      <c r="H74" s="13" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="15">
-      <c r="A75" s="14" t="s">
+    <row r="75" spans="1:8" ht="15">
+      <c r="A75">
+        <v>4</v>
+      </c>
+      <c r="B75" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="C75" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C75" s="5" t="s">
+      <c r="D75" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D75" s="5" t="s">
+      <c r="E75" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E75" s="7"/>
       <c r="F75" s="7"/>
-    </row>
-    <row r="76" spans="1:7">
-      <c r="A76" s="15" t="s">
+      <c r="G75" s="7"/>
+    </row>
+    <row r="76" spans="1:8" ht="14">
+      <c r="A76">
+        <v>0</v>
+      </c>
+      <c r="B76" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="C76" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C76" s="7"/>
       <c r="D76" s="7"/>
       <c r="E76" s="7"/>
       <c r="F76" s="7"/>
-    </row>
-    <row r="77" spans="1:7">
-      <c r="A77" s="15" t="s">
+      <c r="G76" s="7"/>
+    </row>
+    <row r="77" spans="1:8" ht="14">
+      <c r="A77">
+        <v>0</v>
+      </c>
+      <c r="B77" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="C77" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C77" s="7"/>
       <c r="D77" s="7"/>
       <c r="E77" s="7"/>
       <c r="F77" s="7"/>
-    </row>
-    <row r="78" spans="1:7">
-      <c r="A78" s="7" t="s">
+      <c r="G77" s="7"/>
+    </row>
+    <row r="78" spans="1:8" ht="14">
+      <c r="A78">
+        <v>1</v>
+      </c>
+      <c r="B78" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="B78" t="s">
+      <c r="C78" t="s">
         <v>191</v>
       </c>
-      <c r="C78" s="7"/>
       <c r="D78" s="7"/>
       <c r="E78" s="7"/>
       <c r="F78" s="7"/>
+      <c r="G78" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4904,13 +5141,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F24D0452-19E6-4F01-835E-EDFFD925A1F6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F24D0452-19E6-4F01-835E-EDFFD925A1F6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b0dc143a-c2fc-4156-aa7e-afa165885dad"/>
+    <ds:schemaRef ds:uri="7219cb9b-9341-4b3b-a534-b87b88f60fe7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15F7A09C-B649-441E-8760-8D3306812AFA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15F7A09C-B649-441E-8760-8D3306812AFA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7ADE671F-0529-4E8A-8FB0-A73F044F3567}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7ADE671F-0529-4E8A-8FB0-A73F044F3567}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7219cb9b-9341-4b3b-a534-b87b88f60fe7"/>
+    <ds:schemaRef ds:uri="b0dc143a-c2fc-4156-aa7e-afa165885dad"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>